<commit_message>
Selenium Framework for Beginners 19 _ Selenium TestNG How to get data from Excel using DataProvider
</commit_message>
<xml_diff>
--- a/SeleniumFrameWork/excel/data.xlsx
+++ b/SeleniumFrameWork/excel/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -22,16 +22,28 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Admin1</t>
+    <t xml:space="preserve"> Admin </t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
   <si>
     <t>Admin2</t>
   </si>
   <si>
+    <t>admin1234</t>
+  </si>
+  <si>
     <t>Admin3</t>
   </si>
   <si>
+    <t>admin12345</t>
+  </si>
+  <si>
     <t>Admin4</t>
+  </si>
+  <si>
+    <t>admin123456</t>
   </si>
 </sst>
 </file>
@@ -969,7 +981,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -990,29 +1002,32 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>123</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
-      <c r="B3">
-        <v>22</v>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
-      <c r="B4">
-        <v>33</v>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
// Parameterized  data passing to ExcelUtilsab.java in that construct will pick  -Video 18
</commit_message>
<xml_diff>
--- a/SeleniumFrameWork/excel/data.xlsx
+++ b/SeleniumFrameWork/excel/data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -51,10 +52,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -65,6 +66,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -73,38 +82,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,31 +120,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,31 +151,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,37 +225,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,13 +357,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,121 +393,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,21 +410,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -475,17 +461,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -497,6 +472,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,145 +516,145 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -978,13 +979,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="20.0909090909091" customWidth="1"/>
     <col min="2" max="2" width="24.3636363636364" customWidth="1"/>
@@ -1030,8 +1031,108 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>1233</v>
+      </c>
+      <c r="B6">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>